<commit_message>
Relatorio de contas UFS
</commit_message>
<xml_diff>
--- a/2020/contas2020.xlsx
+++ b/2020/contas2020.xlsx
@@ -1,229 +1,251 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vascoalbertofiliperibeiro/R/SUS/2020/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442442FA-59AB-D947-8356-FBE322B05BCD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15620" windowHeight="10460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
-  <si>
-    <t xml:space="preserve">Mês</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DATA.MOV.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DATA.VALOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESCRIÇÃO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMPORTÂNCIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SALDO.CONTABILÍSTICO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CENTRO.DE.CUSTO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RUBRICA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SP-00026322892 SECURITAS DIREC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INSTALAÇÕES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SECURITAS - ALARME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SP-96611566046 Servicos Munici</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSUMO ÁGUA (SMAS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMPRA   LEROY MERLIN SINTRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MANUTENÇÃO / OBRAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMISSÃO MANUTENÇÃO DE CONTA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESP. BANCÁRIAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I.SELO OP.BANC.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SP-00531446107 VODAFONE PORTUG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMUNICAÇÕES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMPRA   IKEA ALFRAGIDE LINHA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARTIGOS DECORATIVOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SP-10367661    MAFEP MATERIAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALUGUER EXTINTORES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRF. PT50001800000671233402153</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOITE DAS CAMÉLIAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OUTROS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SP-P05100001520EDP SERVICO UNI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSUMO ELECTRICIDADE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMPRA   AUCHAN SINTRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMPRA   SINTRA ELECTRICA DE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TR-MUNICIPIO DE SINTRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEATRO UNIÃO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APOIO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMPRA   HIPER CHINA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ATIVIDADES DIVERSAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMPRAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRF. PT50001800032273467702065</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GUARDA ROUPA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRF. PT50000700000032524109823</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SERVIÇO DE LIMPEZA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRF. PT50078101120112001311680</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CERTIDÕES E DECLARAÇÕES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAG.SERV. 11990 411558820</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMPRA   PIRIQUITA 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENCARGOS COM COLABORADORES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMPRA   LEROY MERLIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MANUTENÇÃO/OBRAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRF. PT50003501810000046033029</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TR-EDP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSUMO DE ELECTRICIDADE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRF. PT50003300000000812850405</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IGAC / SPA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRF. PT50003600509910031520496</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GÁS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRF. PT50003300004536624719105</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRODUTOS DE LIMPEZA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TR-UNIAO FREGUESIAS SINTRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAG.SERV. 11034 092254467</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEGUROS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DISPONIB. CARTÃO DÉBITO   7681</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TR-JOSE ANTONIO AZEVEDO UNIPES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAG.ESP.  PAG-ESTADO</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="73">
+  <si>
+    <t>Mês</t>
+  </si>
+  <si>
+    <t>DATA.MOV.</t>
+  </si>
+  <si>
+    <t>DATA.VALOR</t>
+  </si>
+  <si>
+    <t>DESCRIÇÃO</t>
+  </si>
+  <si>
+    <t>IMPORTÂNCIA</t>
+  </si>
+  <si>
+    <t>SALDO.CONTABILÍSTICO</t>
+  </si>
+  <si>
+    <t>CENTRO.DE.CUSTO</t>
+  </si>
+  <si>
+    <t>RUBRICA</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>SP-00026322892 SECURITAS DIREC</t>
+  </si>
+  <si>
+    <t>INSTALAÇÕES</t>
+  </si>
+  <si>
+    <t>SECURITAS - ALARME</t>
+  </si>
+  <si>
+    <t>SP-96611566046 Servicos Munici</t>
+  </si>
+  <si>
+    <t>CONSUMO ÁGUA (SMAS)</t>
+  </si>
+  <si>
+    <t>COMPRA   LEROY MERLIN SINTRA</t>
+  </si>
+  <si>
+    <t>MANUTENÇÃO / OBRAS</t>
+  </si>
+  <si>
+    <t>COMISSÃO MANUTENÇÃO DE CONTA</t>
+  </si>
+  <si>
+    <t>DESP. BANCÁRIAS</t>
+  </si>
+  <si>
+    <t>I.SELO OP.BANC.</t>
+  </si>
+  <si>
+    <t>SP-00531446107 VODAFONE PORTUG</t>
+  </si>
+  <si>
+    <t>COMUNICAÇÕES</t>
+  </si>
+  <si>
+    <t>COMPRA   IKEA ALFRAGIDE LINHA</t>
+  </si>
+  <si>
+    <t>ARTIGOS DECORATIVOS</t>
+  </si>
+  <si>
+    <t>SP-10367661    MAFEP MATERIAL</t>
+  </si>
+  <si>
+    <t>ALUGUER EXTINTORES</t>
+  </si>
+  <si>
+    <t>TRF. PT50001800000671233402153</t>
+  </si>
+  <si>
+    <t>NOITE DAS CAMÉLIAS</t>
+  </si>
+  <si>
+    <t>OUTROS</t>
+  </si>
+  <si>
+    <t>SP-P05100001520EDP SERVICO UNI</t>
+  </si>
+  <si>
+    <t>CONSUMO ELECTRICIDADE</t>
+  </si>
+  <si>
+    <t>COMPRA   AUCHAN SINTRA</t>
+  </si>
+  <si>
+    <t>COMPRA   SINTRA ELECTRICA DE</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>TR-MUNICIPIO DE SINTRA</t>
+  </si>
+  <si>
+    <t>TEATRO UNIÃO</t>
+  </si>
+  <si>
+    <t>APOIO</t>
+  </si>
+  <si>
+    <t>COMPRA   HIPER CHINA</t>
+  </si>
+  <si>
+    <t>ATIVIDADES DIVERSAS</t>
+  </si>
+  <si>
+    <t>COMPRAS</t>
+  </si>
+  <si>
+    <t>TRF. PT50001800032273467702065</t>
+  </si>
+  <si>
+    <t>GUARDA ROUPA</t>
+  </si>
+  <si>
+    <t>TRF. PT50000700000032524109823</t>
+  </si>
+  <si>
+    <t>SERVIÇO DE LIMPEZA</t>
+  </si>
+  <si>
+    <t>TRF. PT50078101120112001311680</t>
+  </si>
+  <si>
+    <t>CERTIDÕES E DECLARAÇÕES</t>
+  </si>
+  <si>
+    <t>PAG.SERV. 11990 411558820</t>
+  </si>
+  <si>
+    <t>COMPRA   PIRIQUITA 1</t>
+  </si>
+  <si>
+    <t>ENCARGOS COM COLABORADORES</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>COMPRA   LEROY MERLIN</t>
+  </si>
+  <si>
+    <t>TRF. PT50003501810000046033029</t>
+  </si>
+  <si>
+    <t>TR-EDP</t>
+  </si>
+  <si>
+    <t>CONSUMO DE ELECTRICIDADE</t>
+  </si>
+  <si>
+    <t>TRF. PT50003300000000812850405</t>
+  </si>
+  <si>
+    <t>IGAC / SPA</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>TRF. PT50003600509910031520496</t>
+  </si>
+  <si>
+    <t>GÁS</t>
+  </si>
+  <si>
+    <t>TRF. PT50003300004536624719105</t>
+  </si>
+  <si>
+    <t>PRODUTOS DE LIMPEZA</t>
+  </si>
+  <si>
+    <t>TR-UNIAO FREGUESIAS SINTRA</t>
+  </si>
+  <si>
+    <t>PAG.SERV. 11034 092254467</t>
+  </si>
+  <si>
+    <t>SEGUROS</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>DISPONIB. CARTÃO DÉBITO   7681</t>
+  </si>
+  <si>
+    <t>TR-JOSE ANTONIO AZEVEDO UNIPES</t>
+  </si>
+  <si>
+    <t>PAG.ESP.  PAG-ESTADO</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>TRF. PT50001000005733259000145</t>
+  </si>
+  <si>
+    <t>COMPRA   LIDL SINTRA ALGUEIRA</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>COMPRA   SECURITY</t>
+  </si>
+  <si>
+    <t>COMPRA   MAX-MAT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -259,12 +281,21 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -546,14 +577,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -579,23 +612,23 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="1">
         <v>43832</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="1">
         <v>43832</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>-50.38</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>5148.91</v>
       </c>
       <c r="G2" t="s">
@@ -605,24 +638,24 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="1">
         <v>43832</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="1">
         <v>43832</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>-19.55</v>
       </c>
-      <c r="F3" t="n">
-        <v>5129.36</v>
+      <c r="F3">
+        <v>5129.3599999999997</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
@@ -631,24 +664,24 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="1">
         <v>43833</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="1">
         <v>43833</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>-53.47</v>
       </c>
-      <c r="F4" t="n">
-        <v>5075.89</v>
+      <c r="F4">
+        <v>5075.8900000000003</v>
       </c>
       <c r="G4" t="s">
         <v>10</v>
@@ -657,24 +690,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="1">
         <v>43833</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="1">
         <v>43833</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
         <v>-5</v>
       </c>
-      <c r="F5" t="n">
-        <v>5070.89</v>
+      <c r="F5">
+        <v>5070.8900000000003</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
@@ -683,24 +716,24 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="1">
         <v>43833</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="1">
         <v>43833</v>
       </c>
       <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>-0.2</v>
       </c>
-      <c r="F6" t="n">
-        <v>5070.69</v>
+      <c r="F6">
+        <v>5070.6899999999996</v>
       </c>
       <c r="G6" t="s">
         <v>10</v>
@@ -709,23 +742,23 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="1">
         <v>43836</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="1">
         <v>43836</v>
       </c>
       <c r="D7" t="s">
         <v>19</v>
       </c>
-      <c r="E7" t="n">
-        <v>-69.93</v>
-      </c>
-      <c r="F7" t="n">
+      <c r="E7">
+        <v>-69.930000000000007</v>
+      </c>
+      <c r="F7">
         <v>5000.76</v>
       </c>
       <c r="G7" t="s">
@@ -735,24 +768,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="1">
         <v>43837</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="1">
         <v>43835</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8">
         <v>-15.9</v>
       </c>
-      <c r="F8" t="n">
-        <v>4984.86</v>
+      <c r="F8">
+        <v>4984.8599999999997</v>
       </c>
       <c r="G8" t="s">
         <v>10</v>
@@ -761,23 +794,23 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="1">
         <v>43838</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C9" s="1">
         <v>43838</v>
       </c>
       <c r="D9" t="s">
         <v>23</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
         <v>-29.52</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9">
         <v>4955.34</v>
       </c>
       <c r="G9" t="s">
@@ -787,24 +820,24 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="n">
+      <c r="B10" s="1">
         <v>43840</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="1">
         <v>43840</v>
       </c>
       <c r="D10" t="s">
         <v>25</v>
       </c>
-      <c r="E10" t="n">
-        <v>-130.95</v>
-      </c>
-      <c r="F10" t="n">
-        <v>4824.39</v>
+      <c r="E10">
+        <v>-130.94999999999999</v>
+      </c>
+      <c r="F10">
+        <v>4824.3900000000003</v>
       </c>
       <c r="G10" t="s">
         <v>26</v>
@@ -813,23 +846,23 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="1">
         <v>43843</v>
       </c>
-      <c r="C11" s="1" t="n">
+      <c r="C11" s="1">
         <v>43843</v>
       </c>
       <c r="D11" t="s">
         <v>28</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11">
         <v>-27.92</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F11">
         <v>4796.47</v>
       </c>
       <c r="G11" t="s">
@@ -839,24 +872,24 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="1">
         <v>43845</v>
       </c>
-      <c r="C12" s="1" t="n">
+      <c r="C12" s="1">
         <v>43845</v>
       </c>
       <c r="D12" t="s">
         <v>28</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E12">
         <v>-209.53</v>
       </c>
-      <c r="F12" t="n">
-        <v>4586.94</v>
+      <c r="F12">
+        <v>4586.9399999999996</v>
       </c>
       <c r="G12" t="s">
         <v>10</v>
@@ -865,23 +898,23 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="B13" s="1">
         <v>43845</v>
       </c>
-      <c r="C13" s="1" t="n">
+      <c r="C13" s="1">
         <v>43845</v>
       </c>
       <c r="D13" t="s">
         <v>30</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E13">
         <v>-10.97</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F13">
         <v>4575.97</v>
       </c>
       <c r="G13" t="s">
@@ -891,23 +924,23 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="B14" s="1">
         <v>43858</v>
       </c>
-      <c r="C14" s="1" t="n">
+      <c r="C14" s="1">
         <v>43858</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
       </c>
-      <c r="E14" t="n">
-        <v>-19.15</v>
-      </c>
-      <c r="F14" t="n">
+      <c r="E14">
+        <v>-19.149999999999999</v>
+      </c>
+      <c r="F14">
         <v>4556.82</v>
       </c>
       <c r="G14" t="s">
@@ -917,23 +950,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="1" t="n">
+      <c r="B15" s="1">
         <v>43858</v>
       </c>
-      <c r="C15" s="1" t="n">
+      <c r="C15" s="1">
         <v>43858</v>
       </c>
       <c r="D15" t="s">
         <v>14</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E15">
         <v>-189.53</v>
       </c>
-      <c r="F15" t="n">
+      <c r="F15">
         <v>4367.29</v>
       </c>
       <c r="G15" t="s">
@@ -943,23 +976,23 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="1" t="n">
+      <c r="B16" s="1">
         <v>43858</v>
       </c>
-      <c r="C16" s="1" t="n">
+      <c r="C16" s="1">
         <v>43858</v>
       </c>
       <c r="D16" t="s">
         <v>31</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E16">
         <v>-30.78</v>
       </c>
-      <c r="F16" t="n">
+      <c r="F16">
         <v>4336.51</v>
       </c>
       <c r="G16" t="s">
@@ -969,23 +1002,23 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="1" t="n">
+      <c r="B17" s="1">
         <v>43863</v>
       </c>
-      <c r="C17" s="1" t="n">
+      <c r="C17" s="1">
         <v>43863</v>
       </c>
       <c r="D17" t="s">
         <v>14</v>
       </c>
-      <c r="E17" t="n">
-        <v>-33.48</v>
-      </c>
-      <c r="F17" t="n">
+      <c r="E17">
+        <v>-33.479999999999997</v>
+      </c>
+      <c r="F17">
         <v>4303.03</v>
       </c>
       <c r="G17" t="s">
@@ -995,24 +1028,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="1" t="n">
+      <c r="B18" s="1">
         <v>43864</v>
       </c>
-      <c r="C18" s="1" t="n">
+      <c r="C18" s="1">
         <v>43864</v>
       </c>
       <c r="D18" t="s">
         <v>9</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E18">
         <v>-50.38</v>
       </c>
-      <c r="F18" t="n">
-        <v>4252.65</v>
+      <c r="F18">
+        <v>4252.6499999999996</v>
       </c>
       <c r="G18" t="s">
         <v>10</v>
@@ -1021,24 +1054,24 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="1" t="n">
+      <c r="B19" s="1">
         <v>43865</v>
       </c>
-      <c r="C19" s="1" t="n">
+      <c r="C19" s="1">
         <v>43865</v>
       </c>
       <c r="D19" t="s">
         <v>33</v>
       </c>
-      <c r="E19" t="n">
+      <c r="E19">
         <v>750</v>
       </c>
-      <c r="F19" t="n">
-        <v>5002.65</v>
+      <c r="F19">
+        <v>5002.6499999999996</v>
       </c>
       <c r="G19" t="s">
         <v>34</v>
@@ -1047,24 +1080,24 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="1" t="n">
+      <c r="B20" s="1">
         <v>43865</v>
       </c>
-      <c r="C20" s="1" t="n">
+      <c r="C20" s="1">
         <v>43865</v>
       </c>
       <c r="D20" t="s">
         <v>16</v>
       </c>
-      <c r="E20" t="n">
+      <c r="E20">
         <v>-5</v>
       </c>
-      <c r="F20" t="n">
-        <v>4997.65</v>
+      <c r="F20">
+        <v>4997.6499999999996</v>
       </c>
       <c r="G20" t="s">
         <v>10</v>
@@ -1073,23 +1106,23 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="1" t="n">
+      <c r="B21" s="1">
         <v>43865</v>
       </c>
-      <c r="C21" s="1" t="n">
+      <c r="C21" s="1">
         <v>43865</v>
       </c>
       <c r="D21" t="s">
         <v>18</v>
       </c>
-      <c r="E21" t="n">
+      <c r="E21">
         <v>-0.2</v>
       </c>
-      <c r="F21" t="n">
+      <c r="F21">
         <v>4997.45</v>
       </c>
       <c r="G21" t="s">
@@ -1099,24 +1132,24 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="1" t="n">
+      <c r="B22" s="1">
         <v>43866</v>
       </c>
-      <c r="C22" s="1" t="n">
+      <c r="C22" s="1">
         <v>43866</v>
       </c>
       <c r="D22" t="s">
         <v>19</v>
       </c>
-      <c r="E22" t="n">
+      <c r="E22">
         <v>-70.89</v>
       </c>
-      <c r="F22" t="n">
-        <v>4926.56</v>
+      <c r="F22">
+        <v>4926.5600000000004</v>
       </c>
       <c r="G22" t="s">
         <v>10</v>
@@ -1125,23 +1158,23 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="1" t="n">
+      <c r="B23" s="1">
         <v>43867</v>
       </c>
-      <c r="C23" s="1" t="n">
+      <c r="C23" s="1">
         <v>43867</v>
       </c>
       <c r="D23" t="s">
         <v>23</v>
       </c>
-      <c r="E23" t="n">
+      <c r="E23">
         <v>-29.52</v>
       </c>
-      <c r="F23" t="n">
+      <c r="F23">
         <v>4897.04</v>
       </c>
       <c r="G23" t="s">
@@ -1151,23 +1184,23 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="1" t="n">
+      <c r="B24" s="1">
         <v>43867</v>
       </c>
-      <c r="C24" s="1" t="n">
+      <c r="C24" s="1">
         <v>43867</v>
       </c>
       <c r="D24" t="s">
         <v>36</v>
       </c>
-      <c r="E24" t="n">
+      <c r="E24">
         <v>-20.05</v>
       </c>
-      <c r="F24" t="n">
+      <c r="F24">
         <v>4876.99</v>
       </c>
       <c r="G24" t="s">
@@ -1177,23 +1210,23 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="1" t="n">
+      <c r="B25" s="1">
         <v>43878</v>
       </c>
-      <c r="C25" s="1" t="n">
+      <c r="C25" s="1">
         <v>43878</v>
       </c>
       <c r="D25" t="s">
         <v>39</v>
       </c>
-      <c r="E25" t="n">
+      <c r="E25">
         <v>-97.53</v>
       </c>
-      <c r="F25" t="n">
+      <c r="F25">
         <v>4779.46</v>
       </c>
       <c r="G25" t="s">
@@ -1203,23 +1236,23 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="1" t="n">
+      <c r="B26" s="1">
         <v>43878</v>
       </c>
-      <c r="C26" s="1" t="n">
+      <c r="C26" s="1">
         <v>43878</v>
       </c>
       <c r="D26" t="s">
         <v>41</v>
       </c>
-      <c r="E26" t="n">
+      <c r="E26">
         <v>-36</v>
       </c>
-      <c r="F26" t="n">
+      <c r="F26">
         <v>4743.46</v>
       </c>
       <c r="G26" t="s">
@@ -1229,23 +1262,23 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="1" t="n">
+      <c r="B27" s="1">
         <v>43882</v>
       </c>
-      <c r="C27" s="1" t="n">
+      <c r="C27" s="1">
         <v>43882</v>
       </c>
       <c r="D27" t="s">
         <v>43</v>
       </c>
-      <c r="E27" t="n">
+      <c r="E27">
         <v>-30</v>
       </c>
-      <c r="F27" t="n">
+      <c r="F27">
         <v>4713.46</v>
       </c>
       <c r="G27" t="s">
@@ -1255,23 +1288,23 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="1" t="n">
+      <c r="B28" s="1">
         <v>43882</v>
       </c>
-      <c r="C28" s="1" t="n">
+      <c r="C28" s="1">
         <v>43882</v>
       </c>
       <c r="D28" t="s">
         <v>14</v>
       </c>
-      <c r="E28" t="n">
+      <c r="E28">
         <v>-19.84</v>
       </c>
-      <c r="F28" t="n">
+      <c r="F28">
         <v>4693.62</v>
       </c>
       <c r="G28" t="s">
@@ -1281,23 +1314,23 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="1" t="n">
+      <c r="B29" s="1">
         <v>43889</v>
       </c>
-      <c r="C29" s="1" t="n">
+      <c r="C29" s="1">
         <v>43889</v>
       </c>
       <c r="D29" t="s">
         <v>12</v>
       </c>
-      <c r="E29" t="n">
+      <c r="E29">
         <v>-20.21</v>
       </c>
-      <c r="F29" t="n">
+      <c r="F29">
         <v>4673.41</v>
       </c>
       <c r="G29" t="s">
@@ -1307,24 +1340,24 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="1" t="n">
+      <c r="B30" s="1">
         <v>43889</v>
       </c>
-      <c r="C30" s="1" t="n">
+      <c r="C30" s="1">
         <v>43889</v>
       </c>
       <c r="D30" t="s">
         <v>45</v>
       </c>
-      <c r="E30" t="n">
+      <c r="E30">
         <v>-393.6</v>
       </c>
-      <c r="F30" t="n">
-        <v>4279.81</v>
+      <c r="F30">
+        <v>4279.8100000000004</v>
       </c>
       <c r="G30" t="s">
         <v>10</v>
@@ -1333,24 +1366,24 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="1" t="n">
+      <c r="B31" s="1">
         <v>43890</v>
       </c>
-      <c r="C31" s="1" t="n">
+      <c r="C31" s="1">
         <v>43890</v>
       </c>
       <c r="D31" t="s">
         <v>46</v>
       </c>
-      <c r="E31" t="n">
+      <c r="E31">
         <v>-7.5</v>
       </c>
-      <c r="F31" t="n">
-        <v>4272.31</v>
+      <c r="F31">
+        <v>4272.3100000000004</v>
       </c>
       <c r="G31" t="s">
         <v>10</v>
@@ -1359,49 +1392,49 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>48</v>
       </c>
-      <c r="B32" s="1" t="n">
+      <c r="B32" s="1">
         <v>43891</v>
       </c>
-      <c r="C32" s="1" t="n">
+      <c r="C32" s="1">
         <v>43891</v>
       </c>
       <c r="D32" t="s">
         <v>49</v>
       </c>
-      <c r="E32" t="n">
+      <c r="E32">
         <v>-14.88</v>
       </c>
-      <c r="F32" t="n">
+      <c r="F32">
         <v>4257.43</v>
       </c>
       <c r="G32" t="s">
         <v>10</v>
       </c>
       <c r="H32" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="1" t="n">
+      <c r="B33" s="1">
         <v>43892</v>
       </c>
-      <c r="C33" s="1" t="n">
+      <c r="C33" s="1">
         <v>43892</v>
       </c>
       <c r="D33" t="s">
         <v>9</v>
       </c>
-      <c r="E33" t="n">
+      <c r="E33">
         <v>-50.38</v>
       </c>
-      <c r="F33" t="n">
+      <c r="F33">
         <v>4207.05</v>
       </c>
       <c r="G33" t="s">
@@ -1411,75 +1444,75 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="1" t="n">
+      <c r="B34" s="1">
         <v>43892</v>
       </c>
-      <c r="C34" s="1" t="n">
+      <c r="C34" s="1">
         <v>43892</v>
       </c>
       <c r="D34" t="s">
-        <v>51</v>
-      </c>
-      <c r="E34" t="n">
+        <v>50</v>
+      </c>
+      <c r="E34">
         <v>-1160</v>
       </c>
-      <c r="F34" t="n">
+      <c r="F34">
         <v>3047.05</v>
       </c>
       <c r="G34" t="s">
         <v>10</v>
       </c>
       <c r="H34" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="1" t="n">
+      <c r="B35" s="1">
         <v>43893</v>
       </c>
-      <c r="C35" s="1" t="n">
+      <c r="C35" s="1">
         <v>43893</v>
       </c>
       <c r="D35" t="s">
+        <v>51</v>
+      </c>
+      <c r="E35">
+        <v>20.29</v>
+      </c>
+      <c r="F35">
+        <v>3067.34</v>
+      </c>
+      <c r="G35" t="s">
+        <v>10</v>
+      </c>
+      <c r="H35" t="s">
         <v>52</v>
       </c>
-      <c r="E35" t="n">
-        <v>20.29</v>
-      </c>
-      <c r="F35" t="n">
-        <v>3067.34</v>
-      </c>
-      <c r="G35" t="s">
-        <v>10</v>
-      </c>
-      <c r="H35" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="36">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="1" t="n">
+      <c r="B36" s="1">
         <v>43893</v>
       </c>
-      <c r="C36" s="1" t="n">
+      <c r="C36" s="1">
         <v>43893</v>
       </c>
       <c r="D36" t="s">
         <v>16</v>
       </c>
-      <c r="E36" t="n">
+      <c r="E36">
         <v>-5</v>
       </c>
-      <c r="F36" t="n">
+      <c r="F36">
         <v>3062.34</v>
       </c>
       <c r="G36" t="s">
@@ -1489,23 +1522,23 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>48</v>
       </c>
-      <c r="B37" s="1" t="n">
+      <c r="B37" s="1">
         <v>43893</v>
       </c>
-      <c r="C37" s="1" t="n">
+      <c r="C37" s="1">
         <v>43893</v>
       </c>
       <c r="D37" t="s">
         <v>18</v>
       </c>
-      <c r="E37" t="n">
+      <c r="E37">
         <v>-0.2</v>
       </c>
-      <c r="F37" t="n">
+      <c r="F37">
         <v>3062.14</v>
       </c>
       <c r="G37" t="s">
@@ -1515,23 +1548,23 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>48</v>
       </c>
-      <c r="B38" s="1" t="n">
+      <c r="B38" s="1">
         <v>43896</v>
       </c>
-      <c r="C38" s="1" t="n">
+      <c r="C38" s="1">
         <v>43896</v>
       </c>
       <c r="D38" t="s">
         <v>23</v>
       </c>
-      <c r="E38" t="n">
+      <c r="E38">
         <v>-29.52</v>
       </c>
-      <c r="F38" t="n">
+      <c r="F38">
         <v>3032.62</v>
       </c>
       <c r="G38" t="s">
@@ -1541,23 +1574,23 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="1" t="n">
+      <c r="B39" s="1">
         <v>43896</v>
       </c>
-      <c r="C39" s="1" t="n">
+      <c r="C39" s="1">
         <v>43896</v>
       </c>
       <c r="D39" t="s">
         <v>19</v>
       </c>
-      <c r="E39" t="n">
+      <c r="E39">
         <v>-80.89</v>
       </c>
-      <c r="F39" t="n">
+      <c r="F39">
         <v>2951.73</v>
       </c>
       <c r="G39" t="s">
@@ -1567,23 +1600,23 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>48</v>
       </c>
-      <c r="B40" s="1" t="n">
+      <c r="B40" s="1">
         <v>43899</v>
       </c>
-      <c r="C40" s="1" t="n">
+      <c r="C40" s="1">
         <v>43899</v>
       </c>
       <c r="D40" t="s">
         <v>14</v>
       </c>
-      <c r="E40" t="n">
+      <c r="E40">
         <v>-155.97</v>
       </c>
-      <c r="F40" t="n">
+      <c r="F40">
         <v>2795.76</v>
       </c>
       <c r="G40" t="s">
@@ -1593,50 +1626,50 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="1" t="n">
+      <c r="B41" s="1">
         <v>43900</v>
       </c>
-      <c r="C41" s="1" t="n">
+      <c r="C41" s="1">
         <v>43900</v>
       </c>
       <c r="D41" t="s">
-        <v>54</v>
-      </c>
-      <c r="E41" t="n">
+        <v>53</v>
+      </c>
+      <c r="E41">
         <v>-28.13</v>
       </c>
-      <c r="F41" t="n">
+      <c r="F41">
         <v>2767.63</v>
       </c>
       <c r="G41" t="s">
         <v>26</v>
       </c>
       <c r="H41" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="42">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="1" t="n">
+      <c r="B42" s="1">
         <v>43906</v>
       </c>
-      <c r="C42" s="1" t="n">
+      <c r="C42" s="1">
         <v>43906</v>
       </c>
       <c r="D42" t="s">
         <v>28</v>
       </c>
-      <c r="E42" t="n">
+      <c r="E42">
         <v>-213.66</v>
       </c>
-      <c r="F42" t="n">
-        <v>2553.97</v>
+      <c r="F42">
+        <v>2553.9699999999998</v>
       </c>
       <c r="G42" t="s">
         <v>10</v>
@@ -1645,23 +1678,23 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="1" t="n">
+      <c r="B43" s="1">
         <v>43916</v>
       </c>
-      <c r="C43" s="1" t="n">
+      <c r="C43" s="1">
         <v>43916</v>
       </c>
       <c r="D43" t="s">
         <v>12</v>
       </c>
-      <c r="E43" t="n">
-        <v>-4.64</v>
-      </c>
-      <c r="F43" t="n">
+      <c r="E43">
+        <v>-4.6399999999999997</v>
+      </c>
+      <c r="F43">
         <v>2549.33</v>
       </c>
       <c r="G43" t="s">
@@ -1671,24 +1704,24 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>56</v>
-      </c>
-      <c r="B44" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B44" s="1">
         <v>43922</v>
       </c>
-      <c r="C44" s="1" t="n">
+      <c r="C44" s="1">
         <v>43922</v>
       </c>
       <c r="D44" t="s">
         <v>9</v>
       </c>
-      <c r="E44" t="n">
+      <c r="E44">
         <v>-50.38</v>
       </c>
-      <c r="F44" t="n">
-        <v>2498.95</v>
+      <c r="F44">
+        <v>2498.9499999999998</v>
       </c>
       <c r="G44" t="s">
         <v>10</v>
@@ -1697,24 +1730,24 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>56</v>
-      </c>
-      <c r="B45" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B45" s="1">
         <v>43923</v>
       </c>
-      <c r="C45" s="1" t="n">
+      <c r="C45" s="1">
         <v>43923</v>
       </c>
       <c r="D45" t="s">
         <v>16</v>
       </c>
-      <c r="E45" t="n">
+      <c r="E45">
         <v>-5</v>
       </c>
-      <c r="F45" t="n">
-        <v>2493.95</v>
+      <c r="F45">
+        <v>2493.9499999999998</v>
       </c>
       <c r="G45" t="s">
         <v>10</v>
@@ -1723,23 +1756,23 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>56</v>
-      </c>
-      <c r="B46" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B46" s="1">
         <v>43923</v>
       </c>
-      <c r="C46" s="1" t="n">
+      <c r="C46" s="1">
         <v>43923</v>
       </c>
       <c r="D46" t="s">
         <v>18</v>
       </c>
-      <c r="E46" t="n">
+      <c r="E46">
         <v>-0.2</v>
       </c>
-      <c r="F46" t="n">
+      <c r="F46">
         <v>2493.75</v>
       </c>
       <c r="G46" t="s">
@@ -1749,23 +1782,23 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>56</v>
-      </c>
-      <c r="B47" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B47" s="1">
         <v>43924</v>
       </c>
-      <c r="C47" s="1" t="n">
+      <c r="C47" s="1">
         <v>43924</v>
       </c>
       <c r="D47" t="s">
         <v>19</v>
       </c>
-      <c r="E47" t="n">
+      <c r="E47">
         <v>-75.84</v>
       </c>
-      <c r="F47" t="n">
+      <c r="F47">
         <v>2417.91</v>
       </c>
       <c r="G47" t="s">
@@ -1775,49 +1808,49 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" s="1">
+        <v>43924</v>
+      </c>
+      <c r="C48" s="1">
+        <v>43924</v>
+      </c>
+      <c r="D48" t="s">
         <v>56</v>
       </c>
-      <c r="B48" s="1" t="n">
+      <c r="E48">
+        <v>-106</v>
+      </c>
+      <c r="F48">
+        <v>2311.91</v>
+      </c>
+      <c r="G48" t="s">
+        <v>10</v>
+      </c>
+      <c r="H48" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>55</v>
+      </c>
+      <c r="B49" s="1">
         <v>43924</v>
       </c>
-      <c r="C48" s="1" t="n">
-        <v>43924</v>
-      </c>
-      <c r="D48" t="s">
-        <v>57</v>
-      </c>
-      <c r="E48" t="n">
-        <v>-106</v>
-      </c>
-      <c r="F48" t="n">
-        <v>2311.91</v>
-      </c>
-      <c r="G48" t="s">
-        <v>10</v>
-      </c>
-      <c r="H48" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="s">
-        <v>56</v>
-      </c>
-      <c r="B49" s="1" t="n">
-        <v>43924</v>
-      </c>
-      <c r="C49" s="1" t="n">
+      <c r="C49" s="1">
         <v>43924</v>
       </c>
       <c r="D49" t="s">
         <v>41</v>
       </c>
-      <c r="E49" t="n">
+      <c r="E49">
         <v>-108</v>
       </c>
-      <c r="F49" t="n">
+      <c r="F49">
         <v>2203.91</v>
       </c>
       <c r="G49" t="s">
@@ -1827,23 +1860,23 @@
         <v>42</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>56</v>
-      </c>
-      <c r="B50" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B50" s="1">
         <v>43928</v>
       </c>
-      <c r="C50" s="1" t="n">
+      <c r="C50" s="1">
         <v>43928</v>
       </c>
       <c r="D50" t="s">
         <v>23</v>
       </c>
-      <c r="E50" t="n">
+      <c r="E50">
         <v>-29.52</v>
       </c>
-      <c r="F50" t="n">
+      <c r="F50">
         <v>2174.39</v>
       </c>
       <c r="G50" t="s">
@@ -1853,76 +1886,76 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>56</v>
-      </c>
-      <c r="B51" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B51" s="1">
         <v>43929</v>
       </c>
-      <c r="C51" s="1" t="n">
+      <c r="C51" s="1">
         <v>43929</v>
       </c>
       <c r="D51" t="s">
+        <v>58</v>
+      </c>
+      <c r="E51">
+        <v>-33.83</v>
+      </c>
+      <c r="F51">
+        <v>2140.56</v>
+      </c>
+      <c r="G51" t="s">
+        <v>10</v>
+      </c>
+      <c r="H51" t="s">
         <v>59</v>
       </c>
-      <c r="E51" t="n">
-        <v>-33.83</v>
-      </c>
-      <c r="F51" t="n">
-        <v>2140.56</v>
-      </c>
-      <c r="G51" t="s">
-        <v>10</v>
-      </c>
-      <c r="H51" t="s">
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="1">
+        <v>43929</v>
+      </c>
+      <c r="C52" s="1">
+        <v>43929</v>
+      </c>
+      <c r="D52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E52">
+        <v>-30.75</v>
+      </c>
+      <c r="F52">
+        <v>2109.81</v>
+      </c>
+      <c r="G52" t="s">
+        <v>10</v>
+      </c>
+      <c r="H52" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" s="1">
+        <v>43930</v>
+      </c>
+      <c r="C53" s="1">
+        <v>43930</v>
+      </c>
+      <c r="D53" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="s">
-        <v>56</v>
-      </c>
-      <c r="B52" s="1" t="n">
-        <v>43929</v>
-      </c>
-      <c r="C52" s="1" t="n">
-        <v>43929</v>
-      </c>
-      <c r="D52" t="s">
-        <v>59</v>
-      </c>
-      <c r="E52" t="n">
-        <v>-30.75</v>
-      </c>
-      <c r="F52" t="n">
-        <v>2109.81</v>
-      </c>
-      <c r="G52" t="s">
-        <v>10</v>
-      </c>
-      <c r="H52" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="s">
-        <v>56</v>
-      </c>
-      <c r="B53" s="1" t="n">
-        <v>43930</v>
-      </c>
-      <c r="C53" s="1" t="n">
-        <v>43930</v>
-      </c>
-      <c r="D53" t="s">
-        <v>61</v>
-      </c>
-      <c r="E53" t="n">
+      <c r="E53">
         <v>2500</v>
       </c>
-      <c r="F53" t="n">
-        <v>4609.81</v>
+      <c r="F53">
+        <v>4609.8100000000004</v>
       </c>
       <c r="G53" t="s">
         <v>37</v>
@@ -1931,49 +1964,49 @@
         <v>35</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>56</v>
-      </c>
-      <c r="B54" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B54" s="1">
         <v>43949</v>
       </c>
-      <c r="C54" s="1" t="n">
+      <c r="C54" s="1">
         <v>43949</v>
       </c>
       <c r="D54" t="s">
+        <v>61</v>
+      </c>
+      <c r="E54">
+        <v>-538.46</v>
+      </c>
+      <c r="F54">
+        <v>4071.35</v>
+      </c>
+      <c r="G54" t="s">
+        <v>10</v>
+      </c>
+      <c r="H54" t="s">
         <v>62</v>
       </c>
-      <c r="E54" t="n">
-        <v>-538.46</v>
-      </c>
-      <c r="F54" t="n">
-        <v>4071.35</v>
-      </c>
-      <c r="G54" t="s">
-        <v>10</v>
-      </c>
-      <c r="H54" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="55">
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>56</v>
-      </c>
-      <c r="B55" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B55" s="1">
         <v>43950</v>
       </c>
-      <c r="C55" s="1" t="n">
+      <c r="C55" s="1">
         <v>43950</v>
       </c>
       <c r="D55" t="s">
         <v>12</v>
       </c>
-      <c r="E55" t="n">
+      <c r="E55">
         <v>-15.23</v>
       </c>
-      <c r="F55" t="n">
+      <c r="F55">
         <v>4056.12</v>
       </c>
       <c r="G55" t="s">
@@ -1983,23 +2016,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>64</v>
-      </c>
-      <c r="B56" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B56" s="1">
         <v>43955</v>
       </c>
-      <c r="C56" s="1" t="n">
+      <c r="C56" s="1">
         <v>43955</v>
       </c>
       <c r="D56" t="s">
         <v>9</v>
       </c>
-      <c r="E56" t="n">
+      <c r="E56">
         <v>-50.38</v>
       </c>
-      <c r="F56" t="n">
+      <c r="F56">
         <v>4005.74</v>
       </c>
       <c r="G56" t="s">
@@ -2009,23 +2042,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>64</v>
-      </c>
-      <c r="B57" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B57" s="1">
         <v>43956</v>
       </c>
-      <c r="C57" s="1" t="n">
+      <c r="C57" s="1">
         <v>43956</v>
       </c>
       <c r="D57" t="s">
         <v>19</v>
       </c>
-      <c r="E57" t="n">
+      <c r="E57">
         <v>-82.53</v>
       </c>
-      <c r="F57" t="n">
+      <c r="F57">
         <v>3923.21</v>
       </c>
       <c r="G57" t="s">
@@ -2035,23 +2068,23 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>64</v>
-      </c>
-      <c r="B58" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B58" s="1">
         <v>43956</v>
       </c>
-      <c r="C58" s="1" t="n">
+      <c r="C58" s="1">
         <v>43956</v>
       </c>
       <c r="D58" t="s">
         <v>16</v>
       </c>
-      <c r="E58" t="n">
+      <c r="E58">
         <v>-5</v>
       </c>
-      <c r="F58" t="n">
+      <c r="F58">
         <v>3918.21</v>
       </c>
       <c r="G58" t="s">
@@ -2061,23 +2094,23 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>64</v>
-      </c>
-      <c r="B59" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B59" s="1">
         <v>43956</v>
       </c>
-      <c r="C59" s="1" t="n">
+      <c r="C59" s="1">
         <v>43956</v>
       </c>
       <c r="D59" t="s">
         <v>18</v>
       </c>
-      <c r="E59" t="n">
+      <c r="E59">
         <v>-0.2</v>
       </c>
-      <c r="F59" t="n">
+      <c r="F59">
         <v>3918.01</v>
       </c>
       <c r="G59" t="s">
@@ -2087,23 +2120,23 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>64</v>
-      </c>
-      <c r="B60" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B60" s="1">
         <v>43958</v>
       </c>
-      <c r="C60" s="1" t="n">
+      <c r="C60" s="1">
         <v>43958</v>
       </c>
       <c r="D60" t="s">
         <v>23</v>
       </c>
-      <c r="E60" t="n">
+      <c r="E60">
         <v>-29.52</v>
       </c>
-      <c r="F60" t="n">
+      <c r="F60">
         <v>3888.49</v>
       </c>
       <c r="G60" t="s">
@@ -2113,23 +2146,23 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>64</v>
-      </c>
-      <c r="B61" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B61" s="1">
         <v>43963</v>
       </c>
-      <c r="C61" s="1" t="n">
+      <c r="C61" s="1">
         <v>43963</v>
       </c>
       <c r="D61" t="s">
         <v>28</v>
       </c>
-      <c r="E61" t="n">
+      <c r="E61">
         <v>-14.81</v>
       </c>
-      <c r="F61" t="n">
+      <c r="F61">
         <v>3873.68</v>
       </c>
       <c r="G61" t="s">
@@ -2139,23 +2172,23 @@
         <v>29</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>64</v>
-      </c>
-      <c r="B62" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B62" s="1">
         <v>43966</v>
       </c>
-      <c r="C62" s="1" t="n">
+      <c r="C62" s="1">
         <v>43966</v>
       </c>
       <c r="D62" t="s">
         <v>28</v>
       </c>
-      <c r="E62" t="n">
+      <c r="E62">
         <v>-205.09</v>
       </c>
-      <c r="F62" t="n">
+      <c r="F62">
         <v>3668.59</v>
       </c>
       <c r="G62" t="s">
@@ -2165,45 +2198,43 @@
         <v>29</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" s="1">
+        <v>43977</v>
+      </c>
+      <c r="C63" s="1">
+        <v>43977</v>
+      </c>
+      <c r="D63" t="s">
         <v>64</v>
       </c>
-      <c r="B63" s="1" t="n">
+      <c r="E63">
+        <v>-17.5</v>
+      </c>
+      <c r="F63">
+        <v>3651.09</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" s="1">
         <v>43977</v>
       </c>
-      <c r="C63" s="1" t="n">
-        <v>43977</v>
-      </c>
-      <c r="D63" t="s">
-        <v>65</v>
-      </c>
-      <c r="E63" t="n">
-        <v>-17.5</v>
-      </c>
-      <c r="F63" t="n">
-        <v>3651.09</v>
-      </c>
-      <c r="G63"/>
-      <c r="H63"/>
-    </row>
-    <row r="64">
-      <c r="A64" t="s">
-        <v>64</v>
-      </c>
-      <c r="B64" s="1" t="n">
-        <v>43977</v>
-      </c>
-      <c r="C64" s="1" t="n">
+      <c r="C64" s="1">
         <v>43977</v>
       </c>
       <c r="D64" t="s">
         <v>18</v>
       </c>
-      <c r="E64" t="n">
+      <c r="E64">
         <v>-0.7</v>
       </c>
-      <c r="F64" t="n">
+      <c r="F64">
         <v>3650.39</v>
       </c>
       <c r="G64" t="s">
@@ -2213,45 +2244,43 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>64</v>
-      </c>
-      <c r="B65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" s="1">
         <v>43978</v>
       </c>
-      <c r="C65" s="1" t="n">
+      <c r="C65" s="1">
         <v>43978</v>
       </c>
       <c r="D65" t="s">
-        <v>66</v>
-      </c>
-      <c r="E65" t="n">
+        <v>65</v>
+      </c>
+      <c r="E65">
         <v>4500</v>
       </c>
-      <c r="F65" t="n">
+      <c r="F65">
         <v>8150.39</v>
       </c>
-      <c r="G65"/>
-      <c r="H65"/>
-    </row>
-    <row r="66">
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>64</v>
-      </c>
-      <c r="B66" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B66" s="1">
         <v>43979</v>
       </c>
-      <c r="C66" s="1" t="n">
+      <c r="C66" s="1">
         <v>43979</v>
       </c>
       <c r="D66" t="s">
         <v>12</v>
       </c>
-      <c r="E66" t="n">
+      <c r="E66">
         <v>-14.11</v>
       </c>
-      <c r="F66" t="n">
+      <c r="F66">
         <v>8136.28</v>
       </c>
       <c r="G66" t="s">
@@ -2261,74 +2290,652 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>64</v>
-      </c>
-      <c r="B67" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B67" s="1">
         <v>43979</v>
       </c>
-      <c r="C67" s="1" t="n">
+      <c r="C67" s="1">
         <v>43979</v>
       </c>
       <c r="D67" t="s">
-        <v>67</v>
-      </c>
-      <c r="E67" t="n">
+        <v>66</v>
+      </c>
+      <c r="E67">
         <v>-250</v>
       </c>
-      <c r="F67" t="n">
+      <c r="F67">
         <v>7886.28</v>
       </c>
-      <c r="G67"/>
-      <c r="H67"/>
-    </row>
-    <row r="68">
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>64</v>
-      </c>
-      <c r="B68" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B68" s="1">
         <v>43981</v>
       </c>
-      <c r="C68" s="1" t="n">
+      <c r="C68" s="1">
         <v>43981</v>
       </c>
       <c r="D68" t="s">
-        <v>67</v>
-      </c>
-      <c r="E68" t="n">
+        <v>66</v>
+      </c>
+      <c r="E68">
         <v>-362.69</v>
       </c>
-      <c r="F68" t="n">
+      <c r="F68">
         <v>7523.59</v>
       </c>
-      <c r="G68"/>
-      <c r="H68"/>
-    </row>
-    <row r="69">
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>64</v>
-      </c>
-      <c r="B69" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B69" s="1">
         <v>43981</v>
       </c>
-      <c r="C69" s="1" t="n">
+      <c r="C69" s="1">
         <v>43981</v>
       </c>
       <c r="D69" t="s">
         <v>14</v>
       </c>
-      <c r="E69" t="n">
+      <c r="E69">
         <v>-180.41</v>
       </c>
-      <c r="F69" t="n">
+      <c r="F69">
         <v>7343.18</v>
       </c>
-      <c r="G69"/>
-      <c r="H69"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>67</v>
+      </c>
+      <c r="B70" s="1">
+        <v>43983</v>
+      </c>
+      <c r="C70" s="1">
+        <v>43983</v>
+      </c>
+      <c r="D70" t="s">
+        <v>9</v>
+      </c>
+      <c r="E70">
+        <v>-50.38</v>
+      </c>
+      <c r="F70">
+        <v>7292.8</v>
+      </c>
+      <c r="G70" t="s">
+        <v>10</v>
+      </c>
+      <c r="H70" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>67</v>
+      </c>
+      <c r="B71" s="1">
+        <v>43983</v>
+      </c>
+      <c r="C71" s="1">
+        <v>43983</v>
+      </c>
+      <c r="D71" t="s">
+        <v>68</v>
+      </c>
+      <c r="E71">
+        <v>-1850</v>
+      </c>
+      <c r="F71">
+        <v>5442.8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>67</v>
+      </c>
+      <c r="B72" s="1">
+        <v>43983</v>
+      </c>
+      <c r="C72" s="1">
+        <v>43983</v>
+      </c>
+      <c r="D72" t="s">
+        <v>68</v>
+      </c>
+      <c r="E72">
+        <v>-1840</v>
+      </c>
+      <c r="F72">
+        <v>3602.8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>67</v>
+      </c>
+      <c r="B73" s="1">
+        <v>43983</v>
+      </c>
+      <c r="C73" s="1">
+        <v>43983</v>
+      </c>
+      <c r="D73" t="s">
+        <v>69</v>
+      </c>
+      <c r="E73">
+        <v>-14.99</v>
+      </c>
+      <c r="F73">
+        <v>3587.81</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>67</v>
+      </c>
+      <c r="B74" s="1">
+        <v>43984</v>
+      </c>
+      <c r="C74" s="1">
+        <v>43984</v>
+      </c>
+      <c r="D74" t="s">
+        <v>16</v>
+      </c>
+      <c r="E74">
+        <v>-5</v>
+      </c>
+      <c r="F74">
+        <v>3582.81</v>
+      </c>
+      <c r="G74" t="s">
+        <v>10</v>
+      </c>
+      <c r="H74" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>67</v>
+      </c>
+      <c r="B75" s="1">
+        <v>43984</v>
+      </c>
+      <c r="C75" s="1">
+        <v>43984</v>
+      </c>
+      <c r="D75" t="s">
+        <v>18</v>
+      </c>
+      <c r="E75">
+        <v>-0.2</v>
+      </c>
+      <c r="F75">
+        <v>3582.61</v>
+      </c>
+      <c r="G75" t="s">
+        <v>10</v>
+      </c>
+      <c r="H75" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>67</v>
+      </c>
+      <c r="B76" s="1">
+        <v>43985</v>
+      </c>
+      <c r="C76" s="1">
+        <v>43985</v>
+      </c>
+      <c r="D76" t="s">
+        <v>19</v>
+      </c>
+      <c r="E76">
+        <v>-73.650000000000006</v>
+      </c>
+      <c r="F76">
+        <v>3508.96</v>
+      </c>
+      <c r="G76" t="s">
+        <v>10</v>
+      </c>
+      <c r="H76" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>67</v>
+      </c>
+      <c r="B77" s="1">
+        <v>43985</v>
+      </c>
+      <c r="C77" s="1">
+        <v>43985</v>
+      </c>
+      <c r="D77" t="s">
+        <v>14</v>
+      </c>
+      <c r="E77">
+        <v>-59.98</v>
+      </c>
+      <c r="F77">
+        <v>3448.98</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>67</v>
+      </c>
+      <c r="B78" s="1">
+        <v>43990</v>
+      </c>
+      <c r="C78" s="1">
+        <v>43990</v>
+      </c>
+      <c r="D78" t="s">
+        <v>23</v>
+      </c>
+      <c r="E78">
+        <v>-29.52</v>
+      </c>
+      <c r="F78">
+        <v>3419.46</v>
+      </c>
+      <c r="G78" t="s">
+        <v>10</v>
+      </c>
+      <c r="H78" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>67</v>
+      </c>
+      <c r="B79" s="1">
+        <v>43995</v>
+      </c>
+      <c r="C79" s="1">
+        <v>43995</v>
+      </c>
+      <c r="D79" t="s">
+        <v>69</v>
+      </c>
+      <c r="E79">
+        <v>-39.99</v>
+      </c>
+      <c r="F79">
+        <v>3379.47</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>67</v>
+      </c>
+      <c r="B80" s="1">
+        <v>43995</v>
+      </c>
+      <c r="C80" s="1">
+        <v>43995</v>
+      </c>
+      <c r="D80" t="s">
+        <v>69</v>
+      </c>
+      <c r="E80">
+        <v>-6.16</v>
+      </c>
+      <c r="F80">
+        <v>3373.31</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>67</v>
+      </c>
+      <c r="B81" s="1">
+        <v>44010</v>
+      </c>
+      <c r="C81" s="1">
+        <v>44010</v>
+      </c>
+      <c r="D81" t="s">
+        <v>14</v>
+      </c>
+      <c r="E81">
+        <v>-53.89</v>
+      </c>
+      <c r="F81">
+        <v>3319.42</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>70</v>
+      </c>
+      <c r="B82" s="1">
+        <v>44013</v>
+      </c>
+      <c r="C82" s="1">
+        <v>44013</v>
+      </c>
+      <c r="D82" t="s">
+        <v>9</v>
+      </c>
+      <c r="E82">
+        <v>-50.38</v>
+      </c>
+      <c r="F82">
+        <v>3269.04</v>
+      </c>
+      <c r="G82" t="s">
+        <v>10</v>
+      </c>
+      <c r="H82" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>70</v>
+      </c>
+      <c r="B83" s="1">
+        <v>44014</v>
+      </c>
+      <c r="C83" s="1">
+        <v>44014</v>
+      </c>
+      <c r="D83" t="s">
+        <v>16</v>
+      </c>
+      <c r="E83">
+        <v>-5</v>
+      </c>
+      <c r="F83">
+        <v>3264.04</v>
+      </c>
+      <c r="G83" t="s">
+        <v>10</v>
+      </c>
+      <c r="H83" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>70</v>
+      </c>
+      <c r="B84" s="1">
+        <v>44014</v>
+      </c>
+      <c r="C84" s="1">
+        <v>44014</v>
+      </c>
+      <c r="D84" t="s">
+        <v>18</v>
+      </c>
+      <c r="E84">
+        <v>-0.2</v>
+      </c>
+      <c r="F84">
+        <v>3263.84</v>
+      </c>
+      <c r="G84" t="s">
+        <v>10</v>
+      </c>
+      <c r="H84" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>70</v>
+      </c>
+      <c r="B85" s="1">
+        <v>44015</v>
+      </c>
+      <c r="C85" s="1">
+        <v>44015</v>
+      </c>
+      <c r="D85" t="s">
+        <v>12</v>
+      </c>
+      <c r="E85">
+        <v>-13.8</v>
+      </c>
+      <c r="F85">
+        <v>3250.04</v>
+      </c>
+      <c r="G85" t="s">
+        <v>10</v>
+      </c>
+      <c r="H85" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>70</v>
+      </c>
+      <c r="B86" s="1">
+        <v>44015</v>
+      </c>
+      <c r="C86" s="1">
+        <v>44015</v>
+      </c>
+      <c r="D86" t="s">
+        <v>71</v>
+      </c>
+      <c r="E86">
+        <v>-37.5</v>
+      </c>
+      <c r="F86">
+        <v>3212.54</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>70</v>
+      </c>
+      <c r="B87" s="1">
+        <v>44018</v>
+      </c>
+      <c r="C87" s="1">
+        <v>44018</v>
+      </c>
+      <c r="D87" t="s">
+        <v>19</v>
+      </c>
+      <c r="E87">
+        <v>-71.83</v>
+      </c>
+      <c r="F87">
+        <v>3140.71</v>
+      </c>
+      <c r="G87" t="s">
+        <v>10</v>
+      </c>
+      <c r="H87" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>70</v>
+      </c>
+      <c r="B88" s="1">
+        <v>44020</v>
+      </c>
+      <c r="C88" s="1">
+        <v>44020</v>
+      </c>
+      <c r="D88" t="s">
+        <v>23</v>
+      </c>
+      <c r="E88">
+        <v>-29.52</v>
+      </c>
+      <c r="F88">
+        <v>3111.19</v>
+      </c>
+      <c r="G88" t="s">
+        <v>10</v>
+      </c>
+      <c r="H88" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>70</v>
+      </c>
+      <c r="B89" s="1">
+        <v>44022</v>
+      </c>
+      <c r="C89" s="1">
+        <v>44022</v>
+      </c>
+      <c r="D89" t="s">
+        <v>28</v>
+      </c>
+      <c r="E89">
+        <v>-14.73</v>
+      </c>
+      <c r="F89">
+        <v>3096.46</v>
+      </c>
+      <c r="G89" t="s">
+        <v>10</v>
+      </c>
+      <c r="H89" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>70</v>
+      </c>
+      <c r="B90" s="1">
+        <v>44026</v>
+      </c>
+      <c r="C90" s="1">
+        <v>44026</v>
+      </c>
+      <c r="D90" t="s">
+        <v>28</v>
+      </c>
+      <c r="E90">
+        <v>-203.49</v>
+      </c>
+      <c r="F90">
+        <v>2892.97</v>
+      </c>
+      <c r="G90" t="s">
+        <v>10</v>
+      </c>
+      <c r="H90" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>70</v>
+      </c>
+      <c r="B91" s="1">
+        <v>44033</v>
+      </c>
+      <c r="C91" s="1">
+        <v>44033</v>
+      </c>
+      <c r="D91" t="s">
+        <v>65</v>
+      </c>
+      <c r="E91">
+        <v>1500</v>
+      </c>
+      <c r="F91">
+        <v>4392.97</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>70</v>
+      </c>
+      <c r="B92" s="1">
+        <v>44036</v>
+      </c>
+      <c r="C92" s="1">
+        <v>44036</v>
+      </c>
+      <c r="D92" t="s">
+        <v>14</v>
+      </c>
+      <c r="E92">
+        <v>-19.97</v>
+      </c>
+      <c r="F92">
+        <v>4373</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>70</v>
+      </c>
+      <c r="B93" s="1">
+        <v>44037</v>
+      </c>
+      <c r="C93" s="1">
+        <v>44037</v>
+      </c>
+      <c r="D93" t="s">
+        <v>72</v>
+      </c>
+      <c r="E93">
+        <v>-80.790000000000006</v>
+      </c>
+      <c r="F93">
+        <v>4292.21</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>70</v>
+      </c>
+      <c r="B94" s="1">
+        <v>44039</v>
+      </c>
+      <c r="C94" s="1">
+        <v>44039</v>
+      </c>
+      <c r="D94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E94">
+        <v>-14.43</v>
+      </c>
+      <c r="F94">
+        <v>4277.78</v>
+      </c>
+      <c r="G94" t="s">
+        <v>10</v>
+      </c>
+      <c r="H94" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>